<commit_message>
Add kraken rule version compare
</commit_message>
<xml_diff>
--- a/doc/Kraken Rule Test Doc/Kraken_rule_templation.xlsx
+++ b/doc/Kraken Rule Test Doc/Kraken_rule_templation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>UI Element</t>
   </si>
@@ -104,6 +104,18 @@
     <t>"Rule1: 
 Rule description: Hidden this field When CapDentalClaimDataEntity.transactionType != "OrthodonticServices"
 RuleName:HidePriorProsthesisPlacement</t>
+  </si>
+  <si>
+    <t>Source4</t>
+  </si>
+  <si>
+    <t>CapDentalBaseClaimData.source4</t>
+  </si>
+  <si>
+    <t>Rule1: 
+Rule description: Field is mandatory 
+RuleName:Source4Mandatory 
+Error Message: Source4is required.</t>
   </si>
 </sst>
 </file>
@@ -1230,13 +1242,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.89166666666667" defaultRowHeight="15" customHeight="1" outlineLevelRow="4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="7.89166666666667" defaultRowHeight="15" customHeight="1" outlineLevelRow="5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="45.0583333333333" customWidth="1"/>
     <col min="2" max="2" width="93.9166666666667" customWidth="1"/>
@@ -1320,6 +1332,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" ht="159" customHeight="1" spans="1:6">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>